<commit_message>
testing: QA testing document updated
</commit_message>
<xml_diff>
--- a/acceptance_qa_testing.xlsx
+++ b/acceptance_qa_testing.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Tolvaj\Documents\Temple\Fall 2022\Projects in CS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Tolvaj\Documents\Temple\Fall 2022\Projects in CS\parking-spot-detector-front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88C8F12-8C1A-4046-9FD7-795E178F0B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7B23B1-E6F8-4047-9C18-B72125D0B62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5355" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Project Name</t>
   </si>
@@ -76,78 +75,7 @@
     <t>Parking Spot Detector</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Install Parking Spot Detector using the Expo Mobile Application
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Follow readme installation instructions.</t>
-    </r>
-  </si>
-  <si>
-    <t>Parking Spot Detector should be installed on your device through the Expo mobile application.</t>
-  </si>
-  <si>
     <t>You should see a successful registration message and return to the sign-in screen to continue logging in.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Login
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Enter the correct login credentials to login to the application.</t>
-    </r>
-  </si>
-  <si>
-    <t>After login in, you should be taken to the home screen. If not successful you should see an error alert message.</t>
-  </si>
-  <si>
-    <r>
-      <t>Test Notification                                    -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Visit https://expo.dev/notifications on your browser. Press the (i) button on the top right of the home screen of the mobile app. Copy the push token ID (including the text: ExponentPushToken[***]). Enter this token into the push notification tool. You may enter a title and message which is optional. To use navigation enter a JSON object like ({"coordinates": [39.98181094459152,-75.15653679830299],"parkingAval":true}) and send the notification. Click on the notification on the mobile device.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">                                                               </t>
-    </r>
-  </si>
-  <si>
-    <t>If you were logged in it should take you to the navigation screen and show your current location along with the parking location. Clicking the navigate to location button should open google maps and start live navigation to the location. If the parkingAval: in JSON is changed to false it will not allow you to use the navigate to location button and the map will change back to default zoom to hide any other locations. (Working on removing the marker if false).</t>
   </si>
   <si>
     <r>
@@ -167,11 +95,143 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t xml:space="preserve">Open the Parking Spot Detector app. 
-Tap sign up, enter the information needed to create an account, and click sign in. </t>
+Tap sign up, enter the information needed to create an account, and Register. </t>
     </r>
   </si>
   <si>
-    <t>May need to remove if not complete in time</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Login
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Enter the correct login credentials that were created during registration to sign in. Click sign in.  (forgot password is currently used to bypass login).</t>
+    </r>
+  </si>
+  <si>
+    <t>After login in, you should be taken to the home screen. If not successful you should see an error alert message. Home screen displays the current account information at the top.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Install Parking Spot Detector using the Expo Mobile Application
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Follow readme installation instructions. Scan the appropriate QR code after installing Expo Go App. Open the app and allow precise location permission.</t>
+    </r>
+  </si>
+  <si>
+    <t>Parking Spot Detector should be installed on your device through the Expo mobile application. It should open to the sign in screen.</t>
+  </si>
+  <si>
+    <t>The Marker information screen should open and show more details. The start driving button should start navigation.</t>
+  </si>
+  <si>
+    <t>It should show the new parking area marker with details on the home screen map (You may have to restart the app for it to appear it is a known bug).</t>
+  </si>
+  <si>
+    <t>It should show your current location and then an alert stating no parking available.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parking Area Screen                                                                                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>When on the home screen the map will show parking areas. You may select a marker and click show more info. When showing more info screen opens you may click start driving to start google maps navigation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Parking Area                                                                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>While on the home screen press the create parking area button. When the create parking area screen is open enter the details needed to create a parking area. Once complete press create parking area.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigation Screen                                                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Clicking on the navigation screen tab and then press navigate to location button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Test Notification                                                                                                   -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Visit https://expo.dev/notifications on your browser. Press the (i) button on the top right of the mobile app's home screen. Copy the push token ID (including the text: ExponentPushToken[***]). Enter this token into the push notification tool. You may enter a title and message which is optional. To use navigation enter a JSON object like ({"coordinates": [39.98181094459152,-75.15653679830299], "parkingAval": true}) on the push notification tool and send the notification. Click on the notification on the mobile device.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">                                                               </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If you were logged in it should take you to the navigation screen and show your current location along with the parking location. Clicking the navigate to location button should open google maps and start live navigation to the location. If the parkingAval: in JSON is changed to false it will not allow you to use the navigate to location button and the map will change back to default zoom to hide any other locations. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Profile Screen                                                                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Press the profile screen tab. It should show some of the data that was entered during registration. Currently, we are working on fixing a bug with the update and delete functionality. Press on the logout button.</t>
+    </r>
+  </si>
+  <si>
+    <t>The logout button should log out to the user and return to the sign-in screen.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +422,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -424,6 +484,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1584,16 +1647,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="31.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="16.28515625" style="1"/>
@@ -1610,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3">
-        <f>COUNTIF(D6:D11,"B")</f>
+        <f>COUNTIF(D6:D15,"B")</f>
         <v>0</v>
       </c>
       <c r="E1" s="4"/>
@@ -1624,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <f>COUNTIF(D6:D11,"P")</f>
+        <f>COUNTIF(D6:D15,"P")</f>
         <v>0</v>
       </c>
       <c r="E2" s="4"/>
@@ -1640,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <f>COUNTIF(D6:D11,"F")</f>
+        <f>COUNTIF(D6:D15,"F")</f>
         <v>0</v>
       </c>
       <c r="E3" s="4"/>
@@ -1663,8 +1726,8 @@
         <v>8</v>
       </c>
       <c r="D5" s="7">
-        <f>COUNTA(D7:D11)/5</f>
-        <v>0.2</v>
+        <f>COUNTA(D7:D15)/5</f>
+        <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
@@ -1683,15 +1746,15 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="67.5" customHeight="1">
+    <row r="7" spans="1:5" ht="105" customHeight="1">
       <c r="A7" s="12">
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -1701,14 +1764,12 @@
         <v>2</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="80.45" customHeight="1">
@@ -1716,35 +1777,85 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:5" ht="204" customHeight="1">
+    <row r="10" spans="1:5" ht="80.45" customHeight="1">
       <c r="A10" s="12">
         <v>4</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:5" ht="126.6" customHeight="1">
+    <row r="11" spans="1:5" ht="121.5" customHeight="1">
       <c r="A11" s="12">
         <v>5</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" ht="121.5" customHeight="1">
+      <c r="A12" s="12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" ht="204" customHeight="1">
+      <c r="A13" s="12">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:5" ht="204" customHeight="1">
+      <c r="A14" s="12">
+        <v>8</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>